<commit_message>
change process, add new filter method for UPPD
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oleg.sharipkin\Documents\UiPath\1cPaymentProccess\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oleg.sharipkin\Documents\UiPath\1C_Payments\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F44A8B6-3C87-4971-BF81-291E36B0E422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74243CA5-7C65-4A0F-9B7B-F53876D2B03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -216,9 +216,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>Оплата по лицевому счету 207319776969 за услуги связи за апрель 2020 согласно счету-акту №</t>
-  </si>
-  <si>
     <t>ArgForBuh_RB</t>
   </si>
   <si>
@@ -232,6 +229,39 @@
   </si>
   <si>
     <t>Argument for running 1C8 proccess</t>
+  </si>
+  <si>
+    <t>Acсount</t>
+  </si>
+  <si>
+    <t>207319776969</t>
+  </si>
+  <si>
+    <t>Оплата по лицевому счету NNNNNN за услуги связи за DDDD года согласно Счёт-акту №</t>
+  </si>
+  <si>
+    <t>NNNNNN - подставляем номер счета из параметра Account. DDDD Вставляем месяц и год акта</t>
+  </si>
+  <si>
+    <t>ResponsibleIs</t>
+  </si>
+  <si>
+    <t>Швайков Евгений Сергеевич</t>
+  </si>
+  <si>
+    <t>Для вставки в поле Ответсвенный в УПП</t>
+  </si>
+  <si>
+    <t>ЗАО "Серволюкс Технолоджис"</t>
+  </si>
+  <si>
+    <t>Для заполнения описания в заявке на оплату</t>
+  </si>
+  <si>
+    <t>CompanyFilter</t>
+  </si>
+  <si>
+    <t>Заполняем фильтр в УППД</t>
   </si>
 </sst>
 </file>
@@ -290,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -301,6 +331,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -618,15 +650,15 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="86.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -674,7 +706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -684,7 +716,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -761,50 +793,83 @@
       <c r="A12" t="s">
         <v>62</v>
       </c>
-      <c r="B12" t="s">
-        <v>63</v>
+      <c r="B12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
         <v>67</v>
-      </c>
-      <c r="C13" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
         <v>68</v>
       </c>
+      <c r="B15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1787,12 +1852,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1829,7 +1894,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1840,7 +1905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1954,7 +2019,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2950,12 +3015,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>